<commit_message>
fix case test 6 - 37- 70
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LATRACCIA00/COOPERATIVA_EDP_LATRACCIA/GEPADIAL/V.2.0.3/report_checklist.xlsx
+++ b/GATEWAY/A1#111LATRACCIA00/COOPERATIVA_EDP_LATRACCIA/GEPADIAL/V.2.0.3/report_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fnicoletti/Sviluppo/it-fse-accreditamento/GATEWAY/A1#111LATRACCIA00/COOPERATIVA_EDP_LATRACCIA/GEPADIAL/V.2.0.3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C134995D-E19F-8F45-BF29-BE78A1C62659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B395FC84-6C07-9F43-BD1F-356344C51DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2119,15 +2119,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.bd53cd5a744eb753a616c6cbd24b96b8f4133a7ceb4c81e58ef17b8f6edda267.e5cc12c9e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>a8835de699310425</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10206.33bf17bb725cf82cb26af86b6e2980631449df4aa4819a4151865f7685893796.117368afc6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-18T09:12:25Z</t>
-  </si>
-  <si>
     <t>286fff4e2762772b</t>
   </si>
   <si>
@@ -2140,16 +2131,25 @@
     <t>2023-04-18T09:26:56Z</t>
   </si>
   <si>
-    <t>11569fa5489edb7</t>
-  </si>
-  <si>
-    <t>2023-04-18T09:30:05Z</t>
-  </si>
-  <si>
     <t>2805af9ee4a25807</t>
   </si>
   <si>
     <t>2023-04-18T09:32:04Z</t>
+  </si>
+  <si>
+    <t>8f66e03f24a66033</t>
+  </si>
+  <si>
+    <t>2023-04-19T15:25:13Z</t>
+  </si>
+  <si>
+    <t>04e6c903aa6489c7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10206.33bf17bb725cf82cb26af86b6e2980631449df4aa4819a4151865f7685893796.d84f55f953^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-19T15:34:39Z</t>
   </si>
 </sst>
 </file>
@@ -4135,7 +4135,7 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
@@ -4580,16 +4580,16 @@
         <v>39</v>
       </c>
       <c r="F15" s="27">
-        <v>45034</v>
+        <v>45035</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>83</v>
@@ -5321,10 +5321,10 @@
         <v>45034</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="I36" s="18" t="s">
         <v>437</v>
@@ -5445,10 +5445,10 @@
         <v>45034</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="H39" s="28" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="I39" s="28" t="s">
         <v>437</v>
@@ -5634,13 +5634,13 @@
         <v>432</v>
       </c>
       <c r="F44" s="17">
-        <v>45034</v>
+        <v>45035</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I44" s="18" t="s">
         <v>437</v>
@@ -5761,10 +5761,10 @@
         <v>45034</v>
       </c>
       <c r="G47" s="28" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="H47" s="28" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="I47" s="28" t="s">
         <v>437</v>

</xml_diff>

<commit_message>
fix test case 6
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111LATRACCIA00/COOPERATIVA_EDP_LATRACCIA/GEPADIAL/V.2.0.3/report_checklist.xlsx
+++ b/GATEWAY/A1#111LATRACCIA00/COOPERATIVA_EDP_LATRACCIA/GEPADIAL/V.2.0.3/report_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fnicoletti/Sviluppo/it-fse-accreditamento/GATEWAY/A1#111LATRACCIA00/COOPERATIVA_EDP_LATRACCIA/GEPADIAL/V.2.0.3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B395FC84-6C07-9F43-BD1F-356344C51DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE3CA40-563A-5C46-8B3F-5DC53EE66201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2143,13 +2143,13 @@
     <t>2023-04-19T15:25:13Z</t>
   </si>
   <si>
-    <t>04e6c903aa6489c7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10206.33bf17bb725cf82cb26af86b6e2980631449df4aa4819a4151865f7685893796.d84f55f953^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-19T15:34:39Z</t>
+    <t>a6ccd15b3de1ef62</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10206.33bf17bb725cf82cb26af86b6e2980631449df4aa4819a4151865f7685893796.cf7a41f586^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-21T17:41:36Z</t>
   </si>
 </sst>
 </file>
@@ -4135,10 +4135,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4580,7 +4580,7 @@
         <v>39</v>
       </c>
       <c r="F15" s="27">
-        <v>45035</v>
+        <v>45037</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>531</v>
@@ -27172,26 +27172,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -27422,32 +27402,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27466,6 +27441,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>